<commit_message>
Incomplete version of calculation of eta
</commit_message>
<xml_diff>
--- a/calendars.xlsx
+++ b/calendars.xlsx
@@ -5,14 +5,14 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nicolas\Drive\UDESA\Taller de Tesis\Papers sugeridos\para revisar\Automatic Splines\codigo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nicolas\Drive\UDESA\Taller de Tesis\Papers sugeridos\para revisar\Automatic Splines\NonParametricTermStructure\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050"/>
   </bookViews>
   <sheets>
-    <sheet name="13-Ago" sheetId="1" r:id="rId1"/>
+    <sheet name="Prices" sheetId="1" r:id="rId1"/>
     <sheet name="AO20" sheetId="2" r:id="rId2"/>
     <sheet name="AA21" sheetId="3" r:id="rId3"/>
     <sheet name="A2E2" sheetId="5" r:id="rId4"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="207">
   <si>
     <t>AO20</t>
   </si>
@@ -70,9 +70,6 @@
     <t>AA46</t>
   </si>
   <si>
-    <t>Precio</t>
-  </si>
-  <si>
     <t>Maturity</t>
   </si>
   <si>
@@ -653,6 +650,12 @@
   </si>
   <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t>Bond</t>
   </si>
 </sst>
 </file>
@@ -738,6 +741,74 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1015,7 +1086,7 @@
   <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A12"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1026,20 +1097,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>206</v>
+      </c>
       <c r="B1" t="s">
+        <v>205</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" t="s">
+        <v>199</v>
+      </c>
+      <c r="E1" t="s">
+        <v>200</v>
+      </c>
+      <c r="F1" t="s">
         <v>11</v>
-      </c>
-      <c r="C1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1" t="s">
-        <v>200</v>
-      </c>
-      <c r="E1" t="s">
-        <v>201</v>
-      </c>
-      <c r="F1" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
@@ -1047,7 +1121,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>2932</v>
+        <v>100.34223134839152</v>
       </c>
       <c r="C2" s="3">
         <v>0.08</v>
@@ -1067,7 +1141,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>2805</v>
+        <v>95.995893223819309</v>
       </c>
       <c r="C3" s="3">
         <v>6.8750000000000006E-2</v>
@@ -1087,7 +1161,7 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>2900</v>
+        <v>99.24709103353868</v>
       </c>
       <c r="C4" s="3">
         <v>8.7499999999999994E-2</v>
@@ -1107,7 +1181,7 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>2619</v>
+        <v>89.630390143737174</v>
       </c>
       <c r="C5" s="3">
         <v>5.6250000000000001E-2</v>
@@ -1127,7 +1201,7 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>2480</v>
+        <v>84.873374401095148</v>
       </c>
       <c r="C6" s="3">
         <v>5.7500000000000002E-2</v>
@@ -1147,7 +1221,7 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>2650</v>
+        <v>90.691307323750863</v>
       </c>
       <c r="C7" s="3">
         <v>7.4999999999999997E-2</v>
@@ -1167,7 +1241,7 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>2410</v>
+        <v>82.477754962354553</v>
       </c>
       <c r="C8" s="3">
         <v>6.8750000000000006E-2</v>
@@ -1187,7 +1261,7 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>3436</v>
+        <v>117.59069130732375</v>
       </c>
       <c r="C9" s="3">
         <v>8.2799999999999999E-2</v>
@@ -1202,7 +1276,7 @@
         <v>48944</v>
       </c>
       <c r="H9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
@@ -1210,7 +1284,7 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>2300</v>
+        <v>78.713210130047912</v>
       </c>
       <c r="C10" s="3">
         <v>7.6249999999999998E-2</v>
@@ -1230,7 +1304,7 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>1560</v>
+        <v>53.388090349075981</v>
       </c>
       <c r="C11" s="3">
         <v>2.5000000000000001E-2</v>
@@ -1245,7 +1319,7 @@
         <v>50770</v>
       </c>
       <c r="H11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.35">
@@ -1253,7 +1327,7 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>2310</v>
+        <v>79.055441478439434</v>
       </c>
       <c r="C12" s="3">
         <v>7.6249999999999998E-2</v>
@@ -1292,21 +1366,21 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B1" t="s">
+        <v>203</v>
+      </c>
+      <c r="C1" t="s">
         <v>202</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>204</v>
-      </c>
-      <c r="C1" t="s">
-        <v>203</v>
-      </c>
-      <c r="D1" t="s">
-        <v>205</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B2" s="5">
         <v>3.81</v>
@@ -1318,7 +1392,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B3" s="7">
         <v>3.81</v>
@@ -1330,7 +1404,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B4" s="5">
         <v>3.81</v>
@@ -1342,7 +1416,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B5" s="7">
         <v>3.81</v>
@@ -1354,7 +1428,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B6" s="5">
         <v>3.81</v>
@@ -1366,7 +1440,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B7" s="7">
         <v>3.81</v>
@@ -1378,7 +1452,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B8" s="5">
         <v>3.81</v>
@@ -1390,7 +1464,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B9" s="7">
         <v>3.81</v>
@@ -1402,7 +1476,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B10" s="5">
         <v>3.81</v>
@@ -1414,7 +1488,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B11" s="7">
         <v>3.81</v>
@@ -1426,7 +1500,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B12" s="5">
         <v>3.81</v>
@@ -1438,7 +1512,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B13" s="7">
         <v>3.81</v>
@@ -1450,7 +1524,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B14" s="5">
         <v>3.81</v>
@@ -1462,7 +1536,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B15" s="7">
         <v>3.81</v>
@@ -1474,7 +1548,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" s="8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B16" s="5">
         <v>3.81</v>
@@ -1486,7 +1560,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" s="9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B17" s="7">
         <v>3.81</v>
@@ -1498,7 +1572,7 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" s="8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B18" s="5">
         <v>3.81</v>
@@ -1510,7 +1584,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" s="9" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B19" s="7">
         <v>3.81</v>
@@ -1522,7 +1596,7 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" s="8" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B20" s="5">
         <v>3.81</v>
@@ -1534,7 +1608,7 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B21" s="7">
         <v>3.81</v>
@@ -1546,7 +1620,7 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" s="8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B22" s="5">
         <v>3.81</v>
@@ -1558,7 +1632,7 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" s="9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B23" s="7">
         <v>3.81</v>
@@ -1570,7 +1644,7 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" s="8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B24" s="5">
         <v>3.81</v>
@@ -1582,7 +1656,7 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" s="9" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B25" s="7">
         <v>3.81</v>
@@ -1594,7 +1668,7 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" s="8" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B26" s="5">
         <v>3.81</v>
@@ -1606,7 +1680,7 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" s="9" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B27" s="7">
         <v>3.81</v>
@@ -1618,7 +1692,7 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" s="8" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B28" s="5">
         <v>3.81</v>
@@ -1630,7 +1704,7 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" s="9" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B29" s="7">
         <v>3.81</v>
@@ -1642,7 +1716,7 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30" s="8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B30" s="5">
         <v>3.81</v>
@@ -1654,7 +1728,7 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31" s="9" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B31" s="7">
         <v>3.81</v>
@@ -1666,7 +1740,7 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32" s="8" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B32" s="5">
         <v>3.81</v>
@@ -1678,7 +1752,7 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33" s="9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B33" s="7">
         <v>3.81</v>
@@ -1690,7 +1764,7 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34" s="8" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B34" s="5">
         <v>3.81</v>
@@ -1702,7 +1776,7 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A35" s="9" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B35" s="7">
         <v>3.81</v>
@@ -1716,7 +1790,7 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A36" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B36" s="5">
         <v>2.5499999999999998</v>
@@ -1728,7 +1802,7 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37" s="9" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B37" s="7">
         <v>2.5499999999999998</v>
@@ -1742,7 +1816,7 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A38" s="8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B38" s="5">
         <v>1.29</v>
@@ -1754,7 +1828,7 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A39" s="9" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B39" s="7">
         <v>1.29</v>
@@ -1789,21 +1863,21 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B1" t="s">
+        <v>203</v>
+      </c>
+      <c r="C1" t="s">
         <v>202</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>204</v>
-      </c>
-      <c r="C1" t="s">
-        <v>203</v>
-      </c>
-      <c r="D1" t="s">
-        <v>205</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="8" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B2" s="5">
         <v>1.25</v>
@@ -1815,7 +1889,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="9" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B3" s="7">
         <v>1.88</v>
@@ -1827,7 +1901,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="8" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B4" s="5">
         <v>1.88</v>
@@ -1839,7 +1913,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="9" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B5" s="7">
         <v>1.88</v>
@@ -1851,7 +1925,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="8" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B6" s="5">
         <v>1.88</v>
@@ -1863,7 +1937,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="9" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B7" s="7">
         <v>1.88</v>
@@ -1875,7 +1949,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" s="8" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B8" s="5">
         <v>1.88</v>
@@ -1887,7 +1961,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" s="9" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B9" s="7">
         <v>1.88</v>
@@ -1899,7 +1973,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" s="8" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B10" s="5">
         <v>1.88</v>
@@ -1911,7 +1985,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" s="9" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B11" s="7">
         <v>1.88</v>
@@ -1923,7 +1997,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" s="8" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B12" s="5">
         <v>1.88</v>
@@ -1935,7 +2009,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" s="9" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B13" s="7">
         <v>1.88</v>
@@ -1947,7 +2021,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" s="8" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B14" s="5">
         <v>1.88</v>
@@ -1959,7 +2033,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" s="9" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B15" s="7">
         <v>1.88</v>
@@ -1971,7 +2045,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" s="8" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B16" s="5">
         <v>1.88</v>
@@ -1983,7 +2057,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" s="9" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B17" s="7">
         <v>1.88</v>
@@ -1995,7 +2069,7 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" s="8" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B18" s="5">
         <v>1.88</v>
@@ -2007,7 +2081,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" s="9" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B19" s="7">
         <v>1.88</v>
@@ -2019,7 +2093,7 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" s="8" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B20" s="5">
         <v>1.88</v>
@@ -2031,7 +2105,7 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" s="9" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B21" s="7">
         <v>1.88</v>
@@ -2043,7 +2117,7 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" s="8" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B22" s="5">
         <v>1.88</v>
@@ -2055,7 +2129,7 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" s="9" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B23" s="7">
         <v>2.63</v>
@@ -2067,7 +2141,7 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" s="8" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B24" s="5">
         <v>2.63</v>
@@ -2081,7 +2155,7 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" s="9" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B25" s="7">
         <v>2.4900000000000002</v>
@@ -2095,7 +2169,7 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" s="8" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B26" s="5">
         <v>2.36</v>
@@ -2109,7 +2183,7 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" s="9" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B27" s="7">
         <v>2.23</v>
@@ -2123,7 +2197,7 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" s="8" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B28" s="5">
         <v>2.1</v>
@@ -2137,7 +2211,7 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" s="9" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B29" s="7">
         <v>1.97</v>
@@ -2151,7 +2225,7 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30" s="8" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B30" s="5">
         <v>1.84</v>
@@ -2165,7 +2239,7 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31" s="9" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B31" s="7">
         <v>1.71</v>
@@ -2179,7 +2253,7 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32" s="8" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B32" s="5">
         <v>1.58</v>
@@ -2193,7 +2267,7 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33" s="9" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B33" s="7">
         <v>1.44</v>
@@ -2207,7 +2281,7 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34" s="8" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B34" s="5">
         <v>1.31</v>
@@ -2221,7 +2295,7 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A35" s="9" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B35" s="7">
         <v>1.18</v>
@@ -2235,7 +2309,7 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A36" s="8" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B36" s="5">
         <v>1.05</v>
@@ -2249,7 +2323,7 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37" s="9" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B37" s="7">
         <v>0.92</v>
@@ -2263,7 +2337,7 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A38" s="8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B38" s="5">
         <v>0.79</v>
@@ -2277,7 +2351,7 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A39" s="9" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B39" s="7">
         <v>0.66</v>
@@ -2291,7 +2365,7 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A40" s="8" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B40" s="5">
         <v>0.53</v>
@@ -2305,7 +2379,7 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A41" s="9" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B41" s="7">
         <v>0.39</v>
@@ -2319,7 +2393,7 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A42" s="8" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B42" s="5">
         <v>0.26</v>
@@ -2333,7 +2407,7 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A43" s="9" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B43" s="7">
         <v>7.0000000000000007E-2</v>
@@ -2368,21 +2442,21 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B1" t="s">
+        <v>203</v>
+      </c>
+      <c r="C1" t="s">
         <v>202</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>204</v>
-      </c>
-      <c r="C1" t="s">
-        <v>203</v>
-      </c>
-      <c r="D1" t="s">
-        <v>205</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B2" s="5">
         <v>3.81</v>
@@ -2394,7 +2468,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B3" s="7">
         <v>3.81</v>
@@ -2406,7 +2480,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B4" s="5">
         <v>3.81</v>
@@ -2418,7 +2492,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B5" s="7">
         <v>3.81</v>
@@ -2430,7 +2504,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B6" s="5">
         <v>3.81</v>
@@ -2442,7 +2516,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B7" s="7">
         <v>3.81</v>
@@ -2454,7 +2528,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" s="8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B8" s="5">
         <v>3.81</v>
@@ -2466,7 +2540,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B9" s="7">
         <v>3.81</v>
@@ -2478,7 +2552,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B10" s="5">
         <v>3.81</v>
@@ -2490,7 +2564,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B11" s="7">
         <v>3.81</v>
@@ -2502,7 +2576,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B12" s="5">
         <v>3.81</v>
@@ -2514,7 +2588,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B13" s="7">
         <v>3.81</v>
@@ -2526,7 +2600,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B14" s="5">
         <v>3.81</v>
@@ -2538,7 +2612,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" s="9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B15" s="7">
         <v>3.81</v>
@@ -2550,7 +2624,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B16" s="5">
         <v>3.81</v>
@@ -2562,7 +2636,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B17" s="7">
         <v>3.81</v>
@@ -2574,7 +2648,7 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" s="8" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B18" s="5">
         <v>3.81</v>
@@ -2586,7 +2660,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" s="9" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B19" s="7">
         <v>3.81</v>
@@ -2598,7 +2672,7 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" s="8" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B20" s="5">
         <v>3.81</v>
@@ -2610,7 +2684,7 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" s="9" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B21" s="7">
         <v>3.81</v>
@@ -2622,7 +2696,7 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" s="8" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B22" s="5">
         <v>3.81</v>
@@ -2634,7 +2708,7 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" s="9" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B23" s="7">
         <v>3.81</v>
@@ -2646,7 +2720,7 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" s="8" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B24" s="5">
         <v>3.81</v>
@@ -2658,7 +2732,7 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" s="9" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B25" s="7">
         <v>3.81</v>
@@ -2670,7 +2744,7 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" s="8" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B26" s="5">
         <v>3.81</v>
@@ -2682,7 +2756,7 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" s="9" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B27" s="7">
         <v>3.81</v>
@@ -2694,7 +2768,7 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" s="8" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B28" s="5">
         <v>3.81</v>
@@ -2706,7 +2780,7 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" s="9" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B29" s="7">
         <v>3.81</v>
@@ -2718,7 +2792,7 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30" s="8" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B30" s="5">
         <v>3.81</v>
@@ -2730,7 +2804,7 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31" s="9" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B31" s="7">
         <v>3.81</v>
@@ -2742,7 +2816,7 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32" s="8" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B32" s="5">
         <v>3.81</v>
@@ -2754,7 +2828,7 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33" s="9" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B33" s="7">
         <v>3.81</v>
@@ -2766,7 +2840,7 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34" s="8" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B34" s="5">
         <v>3.81</v>
@@ -2778,7 +2852,7 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A35" s="9" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B35" s="7">
         <v>3.81</v>
@@ -2790,7 +2864,7 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A36" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B36" s="5">
         <v>3.81</v>
@@ -2802,7 +2876,7 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37" s="9" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B37" s="7">
         <v>3.81</v>
@@ -2814,7 +2888,7 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A38" s="8" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B38" s="5">
         <v>3.81</v>
@@ -2826,7 +2900,7 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A39" s="9" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B39" s="7">
         <v>3.81</v>
@@ -2838,7 +2912,7 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A40" s="8" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B40" s="5">
         <v>3.81</v>
@@ -2850,7 +2924,7 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A41" s="9" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B41" s="7">
         <v>3.81</v>
@@ -2862,7 +2936,7 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A42" s="8" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B42" s="5">
         <v>3.81</v>
@@ -2874,7 +2948,7 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A43" s="9" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B43" s="7">
         <v>3.81</v>
@@ -2886,7 +2960,7 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A44" s="8" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B44" s="5">
         <v>3.81</v>
@@ -2898,7 +2972,7 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A45" s="9" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B45" s="7">
         <v>3.81</v>
@@ -2910,7 +2984,7 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A46" s="8" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B46" s="5">
         <v>3.81</v>
@@ -2922,7 +2996,7 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A47" s="9" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B47" s="7">
         <v>3.81</v>
@@ -2934,7 +3008,7 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A48" s="8" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B48" s="5">
         <v>3.81</v>
@@ -2946,7 +3020,7 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A49" s="9" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B49" s="7">
         <v>3.81</v>
@@ -2958,7 +3032,7 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A50" s="8" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B50" s="5">
         <v>3.81</v>
@@ -2970,7 +3044,7 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A51" s="9" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B51" s="7">
         <v>3.81</v>
@@ -2982,7 +3056,7 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A52" s="8" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B52" s="5">
         <v>3.81</v>
@@ -2994,7 +3068,7 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A53" s="9" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B53" s="7">
         <v>3.81</v>
@@ -3006,7 +3080,7 @@
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A54" s="8" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B54" s="5">
         <v>3.81</v>
@@ -3018,7 +3092,7 @@
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A55" s="9" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B55" s="7">
         <v>3.81</v>
@@ -3030,7 +3104,7 @@
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A56" s="8" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B56" s="5">
         <v>3.81</v>
@@ -3042,7 +3116,7 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A57" s="9" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B57" s="7">
         <v>3.81</v>
@@ -3075,16 +3149,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B1" t="s">
+        <v>203</v>
+      </c>
+      <c r="C1" t="s">
         <v>202</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>204</v>
-      </c>
-      <c r="C1" t="s">
-        <v>203</v>
-      </c>
-      <c r="D1" t="s">
-        <v>205</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
@@ -3170,21 +3244,21 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B1" t="s">
+        <v>203</v>
+      </c>
+      <c r="C1" t="s">
         <v>202</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>204</v>
-      </c>
-      <c r="C1" t="s">
-        <v>203</v>
-      </c>
-      <c r="D1" t="s">
-        <v>205</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B2" s="5">
         <v>3.44</v>
@@ -3196,7 +3270,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B3" s="7">
         <v>3.44</v>
@@ -3208,7 +3282,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B4" s="5">
         <v>3.44</v>
@@ -3220,7 +3294,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B5" s="7">
         <v>3.44</v>
@@ -3232,7 +3306,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B6" s="5">
         <v>3.44</v>
@@ -3244,7 +3318,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B7" s="7">
         <v>3.44</v>
@@ -3277,21 +3351,21 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B1" t="s">
+        <v>203</v>
+      </c>
+      <c r="C1" t="s">
         <v>202</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>204</v>
-      </c>
-      <c r="C1" t="s">
-        <v>203</v>
-      </c>
-      <c r="D1" t="s">
-        <v>205</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B2" s="5">
         <v>2.81</v>
@@ -3303,7 +3377,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B3" s="7">
         <v>2.81</v>
@@ -3315,7 +3389,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B4" s="5">
         <v>2.81</v>
@@ -3327,7 +3401,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B5" s="7">
         <v>2.81</v>
@@ -3339,7 +3413,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B6" s="5">
         <v>2.81</v>
@@ -3351,7 +3425,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B7" s="7">
         <v>2.81</v>
@@ -3363,7 +3437,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B8" s="5">
         <v>2.81</v>
@@ -3395,16 +3469,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B1" t="s">
+        <v>203</v>
+      </c>
+      <c r="C1" t="s">
         <v>202</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>204</v>
-      </c>
-      <c r="C1" t="s">
-        <v>203</v>
-      </c>
-      <c r="D1" t="s">
-        <v>205</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
@@ -3583,21 +3657,21 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B1" t="s">
+        <v>203</v>
+      </c>
+      <c r="C1" t="s">
         <v>202</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>204</v>
-      </c>
-      <c r="C1" t="s">
-        <v>203</v>
-      </c>
-      <c r="D1" t="s">
-        <v>205</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B2" s="5">
         <v>2.88</v>
@@ -3609,7 +3683,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B3" s="7">
         <v>2.88</v>
@@ -3621,7 +3695,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B4" s="5">
         <v>2.88</v>
@@ -3633,7 +3707,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B5" s="7">
         <v>2.88</v>
@@ -3645,7 +3719,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B6" s="5">
         <v>2.88</v>
@@ -3657,7 +3731,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B7" s="7">
         <v>2.88</v>
@@ -3669,7 +3743,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B8" s="5">
         <v>2.88</v>
@@ -3681,7 +3755,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B9" s="7">
         <v>2.88</v>
@@ -3693,7 +3767,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B10" s="5">
         <v>2.88</v>
@@ -3705,7 +3779,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B11" s="7">
         <v>2.88</v>
@@ -3719,7 +3793,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B12" s="5">
         <v>1.93</v>
@@ -3731,7 +3805,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B13" s="7">
         <v>1.93</v>
@@ -3745,7 +3819,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B14" s="5">
         <v>0.98</v>
@@ -3757,7 +3831,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B15" s="7">
         <v>0.98</v>
@@ -3790,21 +3864,21 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B1" t="s">
+        <v>203</v>
+      </c>
+      <c r="C1" t="s">
         <v>202</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>204</v>
-      </c>
-      <c r="C1" t="s">
-        <v>203</v>
-      </c>
-      <c r="D1" t="s">
-        <v>205</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B2" s="5">
         <v>3.75</v>
@@ -3816,7 +3890,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B3" s="7">
         <v>3.75</v>
@@ -3828,7 +3902,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B4" s="5">
         <v>3.75</v>
@@ -3840,7 +3914,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B5" s="7">
         <v>3.75</v>
@@ -3852,7 +3926,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B6" s="5">
         <v>3.75</v>
@@ -3864,7 +3938,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B7" s="7">
         <v>3.75</v>
@@ -3876,7 +3950,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" s="8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B8" s="5">
         <v>3.75</v>
@@ -3888,7 +3962,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B9" s="7">
         <v>3.75</v>
@@ -3900,7 +3974,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B10" s="5">
         <v>3.75</v>
@@ -3912,7 +3986,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B11" s="7">
         <v>3.75</v>
@@ -3924,7 +3998,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B12" s="5">
         <v>3.75</v>
@@ -3936,7 +4010,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B13" s="7">
         <v>3.75</v>
@@ -3948,7 +4022,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B14" s="5">
         <v>3.75</v>
@@ -3960,7 +4034,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" s="9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B15" s="7">
         <v>3.75</v>
@@ -3972,7 +4046,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B16" s="5">
         <v>3.75</v>
@@ -3984,7 +4058,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B17" s="7">
         <v>3.75</v>
@@ -4019,21 +4093,21 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B1" t="s">
+        <v>203</v>
+      </c>
+      <c r="C1" t="s">
         <v>202</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>204</v>
-      </c>
-      <c r="C1" t="s">
-        <v>203</v>
-      </c>
-      <c r="D1" t="s">
-        <v>205</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B2" s="5">
         <v>3.44</v>
@@ -4045,7 +4119,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B3" s="7">
         <v>3.44</v>
@@ -4057,7 +4131,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B4" s="5">
         <v>3.44</v>
@@ -4069,7 +4143,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B5" s="7">
         <v>3.44</v>
@@ -4081,7 +4155,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B6" s="5">
         <v>3.44</v>
@@ -4093,7 +4167,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B7" s="7">
         <v>3.44</v>
@@ -4105,7 +4179,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B8" s="5">
         <v>3.44</v>
@@ -4117,7 +4191,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" s="9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B9" s="7">
         <v>3.44</v>
@@ -4129,7 +4203,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B10" s="5">
         <v>3.44</v>
@@ -4141,7 +4215,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" s="9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B11" s="7">
         <v>3.44</v>
@@ -4153,7 +4227,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B12" s="5">
         <v>3.44</v>
@@ -4165,7 +4239,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" s="9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B13" s="7">
         <v>3.44</v>
@@ -4177,7 +4251,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B14" s="5">
         <v>3.44</v>
@@ -4189,7 +4263,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" s="9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B15" s="7">
         <v>3.44</v>
@@ -4201,7 +4275,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" s="8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B16" s="5">
         <v>3.44</v>
@@ -4213,7 +4287,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B17" s="7">
         <v>3.44</v>
@@ -4225,7 +4299,7 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B18" s="5">
         <v>3.44</v>
@@ -4257,21 +4331,21 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B1" t="s">
+        <v>203</v>
+      </c>
+      <c r="C1" t="s">
         <v>202</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>204</v>
-      </c>
-      <c r="C1" t="s">
-        <v>203</v>
-      </c>
-      <c r="D1" t="s">
-        <v>205</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B2" s="5">
         <v>5.8</v>
@@ -4283,7 +4357,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B3" s="7">
         <v>5.8</v>
@@ -4295,7 +4369,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B4" s="5">
         <v>5.8</v>
@@ -4307,7 +4381,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B5" s="7">
         <v>5.8</v>
@@ -4319,7 +4393,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B6" s="5">
         <v>5.8</v>
@@ -4331,7 +4405,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B7" s="7">
         <v>5.8</v>
@@ -4343,7 +4417,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" s="8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B8" s="5">
         <v>5.8</v>
@@ -4355,7 +4429,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B9" s="7">
         <v>5.8</v>
@@ -4367,7 +4441,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" s="8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B10" s="5">
         <v>5.8</v>
@@ -4379,7 +4453,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" s="9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B11" s="7">
         <v>5.8</v>
@@ -4391,7 +4465,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B12" s="5">
         <v>5.8</v>
@@ -4403,7 +4477,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B13" s="7">
         <v>5.8</v>
@@ -4417,7 +4491,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B14" s="5">
         <v>5.51</v>
@@ -4431,7 +4505,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" s="9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B15" s="7">
         <v>5.22</v>
@@ -4445,7 +4519,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" s="8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B16" s="5">
         <v>4.93</v>
@@ -4459,7 +4533,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" s="9" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B17" s="7">
         <v>4.6399999999999997</v>
@@ -4473,7 +4547,7 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" s="8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B18" s="5">
         <v>4.3499999999999996</v>
@@ -4487,7 +4561,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B19" s="7">
         <v>4.0599999999999996</v>
@@ -4501,7 +4575,7 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" s="8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B20" s="5">
         <v>3.77</v>
@@ -4515,7 +4589,7 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" s="9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B21" s="7">
         <v>3.48</v>
@@ -4529,7 +4603,7 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B22" s="5">
         <v>3.19</v>
@@ -4543,7 +4617,7 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" s="9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B23" s="7">
         <v>2.9</v>
@@ -4557,7 +4631,7 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B24" s="5">
         <v>2.61</v>
@@ -4571,7 +4645,7 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" s="9" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B25" s="7">
         <v>2.3199999999999998</v>
@@ -4585,7 +4659,7 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" s="8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B26" s="5">
         <v>2.0299999999999998</v>
@@ -4599,7 +4673,7 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" s="9" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B27" s="7">
         <v>1.74</v>
@@ -4613,7 +4687,7 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" s="8" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B28" s="5">
         <v>1.45</v>
@@ -4627,7 +4701,7 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" s="9" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B29" s="7">
         <v>1.1599999999999999</v>
@@ -4641,7 +4715,7 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B30" s="5">
         <v>0.87</v>
@@ -4655,7 +4729,7 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31" s="9" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B31" s="7">
         <v>0.57999999999999996</v>
@@ -4669,7 +4743,7 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32" s="8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B32" s="5">
         <v>0.28999999999999998</v>

</xml_diff>